<commit_message>
TestScript Added : Create Contact with Organisation
</commit_message>
<xml_diff>
--- a/com.TestYantra.Vtiger.Framework/src/test/resources/testdata.xlsx
+++ b/com.TestYantra.Vtiger.Framework/src/test/resources/testdata.xlsx
@@ -2,16 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\git\Vtiger_Selenium_Framework\com.TestYantra.Vtiger.Framework\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10730" windowHeight="3580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10728" windowHeight="3576"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
     <sheet name="contact" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,20 +426,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="A7:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -447,7 +451,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -459,8 +463,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,7 +477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -488,8 +491,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,14 +504,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -535,10 +536,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>

</xml_diff>